<commit_message>
Updated for seperate the P2P process
</commit_message>
<xml_diff>
--- a/COD R12 Cloud ERP Automation/src/test/resources/TestArtifacts/COD R12 Cloud ERP BatchSheet.xlsx
+++ b/COD R12 Cloud ERP Automation/src/test/resources/TestArtifacts/COD R12 Cloud ERP BatchSheet.xlsx
@@ -47,12 +47,6 @@
     <t>LoginLogout.logout</t>
   </si>
   <si>
-    <t>Cloud.createItemBasedRequisition</t>
-  </si>
-  <si>
-    <t>Cloud.createPurchaseOrder</t>
-  </si>
-  <si>
     <t>Cloud.createInvioce</t>
   </si>
   <si>
@@ -62,15 +56,6 @@
     <t>Cloud.createPaymentInvoice</t>
   </si>
   <si>
-    <t>Cloud.createReceivingReceipt</t>
-  </si>
-  <si>
-    <t>Cloud.createPurOrderMatchedInvoice</t>
-  </si>
-  <si>
-    <t>Cloud.createPaymentQuickCheck</t>
-  </si>
-  <si>
     <t>PO_Create_Purchase_Requisition</t>
   </si>
   <si>
@@ -96,6 +81,21 @@
   </si>
   <si>
     <t>AP_Create_Payment_Invoice</t>
+  </si>
+  <si>
+    <t>P2P.createItemBasedRequisition</t>
+  </si>
+  <si>
+    <t>P2P.createPurchaseOrder</t>
+  </si>
+  <si>
+    <t>P2P.createReceivingReceipt</t>
+  </si>
+  <si>
+    <t>P2P.createPurOrderMatchedInvoice</t>
+  </si>
+  <si>
+    <t>P2P.createPaymentQuickCheck</t>
   </si>
 </sst>
 </file>
@@ -984,7 +984,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -1033,7 +1033,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -1054,7 +1054,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>9</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
@@ -1075,7 +1075,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>9</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -1096,7 +1096,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>9</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -1117,7 +1117,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>9</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -1138,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -1159,7 +1159,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>9</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -1180,7 +1180,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>9</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
@@ -1201,7 +1201,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
updated while giving training to ziya
</commit_message>
<xml_diff>
--- a/COD R12 Cloud ERP Automation/src/test/resources/TestArtifacts/COD R12 Cloud ERP BatchSheet.xlsx
+++ b/COD R12 Cloud ERP Automation/src/test/resources/TestArtifacts/COD R12 Cloud ERP BatchSheet.xlsx
@@ -83,19 +83,19 @@
     <t>AP_Create_Payment_Invoice</t>
   </si>
   <si>
-    <t>P2P.createItemBasedRequisition</t>
-  </si>
-  <si>
-    <t>P2P.createPurchaseOrder</t>
-  </si>
-  <si>
-    <t>P2P.createReceivingReceipt</t>
-  </si>
-  <si>
-    <t>P2P.createPurOrderMatchedInvoice</t>
-  </si>
-  <si>
-    <t>P2P.createPaymentQuickCheck</t>
+    <t>Cloud.createItemBasedRequisition</t>
+  </si>
+  <si>
+    <t>Cloud.createPurchaseOrder</t>
+  </si>
+  <si>
+    <t>Cloud.createReceivingReceipt</t>
+  </si>
+  <si>
+    <t>Cloud.createPurOrderMatchedInvoice</t>
+  </si>
+  <si>
+    <t>Cloud.createPaymentQuickCheck</t>
   </si>
 </sst>
 </file>
@@ -984,7 +984,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>